<commit_message>
Actualización de los planes y schedules
</commit_message>
<xml_diff>
--- a/tspi/ciclo-3/plan3-20105627.xlsx
+++ b/tspi/ciclo-3/plan3-20105627.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecvasro\workspace\pucmm\isc-434-t\ppr\tspi\ciclo-3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="task" sheetId="2" r:id="rId2"/>
     <sheet name="logt" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Id</t>
   </si>
@@ -84,25 +89,10 @@
     <t>Definir la estrategía de desarrolo del ciclo #3 de TSPi.</t>
   </si>
   <si>
-    <t>Elaborar el plan del ciclo #3 de TSPi.</t>
-  </si>
-  <si>
-    <t>Completar el mockup de la vista de calendarización.</t>
-  </si>
-  <si>
     <t>Elaborar el mockup de la vista para la asignación de la disponibilidad de los recursos.</t>
   </si>
   <si>
     <t>Elaborar el mockup de la vista para ver la calendarización de uno o más recursos.</t>
-  </si>
-  <si>
-    <t>Elaborar el pseudocódigo del algoritmo de calendarización.</t>
-  </si>
-  <si>
-    <t>Elaborar el algoritmo de construcción del grafo a partir del archivo csv.</t>
-  </si>
-  <si>
-    <t>Configurar el repositorio global de la aplicación.</t>
   </si>
   <si>
     <t>Crear la agenda para la reunión #4 con el cliente.</t>
@@ -111,18 +101,126 @@
     <t>Reunión #4 con el cliente.</t>
   </si>
   <si>
-    <t>Configurar el repositorio local de la aplicación.</t>
+    <t>Realizar el lanzamiento del ciclo #3.</t>
+  </si>
+  <si>
+    <t>Cada miembro del equipo completó la forma INFO. El equipo llego a un acuerdo con los goles del ciclo 1 y la fecha en que serán entregados los reportes semanales.</t>
+  </si>
+  <si>
+    <t>Definir la estrategía de desarrolo del ciclo #3.</t>
+  </si>
+  <si>
+    <t>El equipo estimó el tamaño y el tiempo de producción de los elementos a producir en el ciclo #1. El equipo definió actualizó el diseño conceptual del proyecto y completó la forma STRAT. El equipo actualizó el documento los riesgos y problemas.</t>
+  </si>
+  <si>
+    <t>Elaborar el plan del ciclo #3.</t>
+  </si>
+  <si>
+    <t>Se completaron las formas TASK y SCHEDULE para el equipo y cada miembro de este. El equipo completo las formas SUMP, SUMQ y SUMS.</t>
+  </si>
+  <si>
+    <t>Elaborar el mokcup de la vista para la creación de un proyecto.</t>
+  </si>
+  <si>
+    <t>Se elaboró el mockup de la vista para la creación de un proyecto.</t>
+  </si>
+  <si>
+    <t>Se elaboró el mockup de la vista para la asignación de la disponibilidad de los recursos.</t>
+  </si>
+  <si>
+    <t>Se elaboró el mockup de la vista para ver la calendarización de uno o más recursos.</t>
+  </si>
+  <si>
+    <t>Se creó la agenda para la reunión #4 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se creó la minuta de la reunión #4 con el cliente.</t>
+  </si>
+  <si>
+    <t>Elaborar el mockup de la vista para ver los eventos o excepciones de los recursos.</t>
+  </si>
+  <si>
+    <t>Se elaboró el mockup de la vista para ver los eventos o excepciones de los recursos.</t>
+  </si>
+  <si>
+    <t>Calcular el tiempo de corrida del algoritmo de calendarización.</t>
+  </si>
+  <si>
+    <t>Se documentó el tiempo de corrida del algoritmo de calendarización.</t>
+  </si>
+  <si>
+    <t>Elaborar el pseudocódigo del algoritmo de construcción de la estructura de calendarización a partir del archivo CSV.</t>
+  </si>
+  <si>
+    <t>Se elaboró el pseudocódigo del algoritmo de construcción de la estructura de calendarización a partir del archivo CSV.</t>
+  </si>
+  <si>
+    <t>Configurar el ambiente global de desarrollo.</t>
+  </si>
+  <si>
+    <t>Se elaboró una guía con todos los pasos para la configuración del ambiente global de desarrollo.</t>
+  </si>
+  <si>
+    <t>Configurar el ambiente local de desarrollo.</t>
+  </si>
+  <si>
+    <t>Cada miembro del equipo configuró su ambiente local de desarrollo.</t>
+  </si>
+  <si>
+    <t>Elaborar el plan de calidad.</t>
+  </si>
+  <si>
+    <t>Elaborar la versión final del diagrama de flujo del algoritmo de calendarización.</t>
+  </si>
+  <si>
+    <t>Se elaboró la versión final del diagrama de flujo del algoritmo de calendarización.</t>
+  </si>
+  <si>
+    <t>Elaborar la versión final del modelo físico de data.</t>
+  </si>
+  <si>
+    <t>Se elaboró la versión final del modelo físico de data.</t>
+  </si>
+  <si>
+    <t>Elaborar la versión final del diagrama de contexto de la arquitectura.</t>
+  </si>
+  <si>
+    <t>Se elaboró la versión final del diagrama de contexto de la arquitectura.</t>
+  </si>
+  <si>
+    <t>Crear la versión final del documento de arquitectura.</t>
+  </si>
+  <si>
+    <t>Se creó la versión final del documento de arquitectura.</t>
+  </si>
+  <si>
+    <t>Crear la agenda para la reunión #5 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se creó la agenda para la reunión #5 con el cliente.</t>
+  </si>
+  <si>
+    <t>Reunión #5 con el cliente.</t>
+  </si>
+  <si>
+    <t>Se creó la minuta de la reunión #5 con el cliente.</t>
+  </si>
+  <si>
+    <t>Elaborar el reporte de cierre del ciclo #3.</t>
+  </si>
+  <si>
+    <t>Cada miembro del equipo completó la forma PEER. Se creó el reporte del ciclo correspondiente. Se completaron las formas SUMP y SUMQ para el sistema y todos sus componentes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -348,11 +446,19 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -394,7 +500,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,9 +532,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,6 +567,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -635,14 +743,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="7" customWidth="1"/>
@@ -654,7 +762,7 @@
     <col min="1014" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1013" s="3" customFormat="1" ht="42.75">
+    <row r="1" spans="1:1013" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,18 +798,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1013" ht="25.5">
-      <c r="A2" s="8">
+    <row r="2" spans="1:1013" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>46</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E2" s="10">
         <v>5</v>
@@ -1727,18 +1835,18 @@
       <c r="ALX2" s="4"/>
       <c r="ALY2" s="4"/>
     </row>
-    <row r="3" spans="1:1013" ht="25.5">
-      <c r="A3" s="8">
+    <row r="3" spans="1:1013" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>47</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="E3" s="10">
         <v>5</v>
@@ -2764,18 +2872,18 @@
       <c r="ALX3" s="4"/>
       <c r="ALY3" s="4"/>
     </row>
-    <row r="4" spans="1:1013">
-      <c r="A4" s="8">
+    <row r="4" spans="1:1013" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>48</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E4" s="10">
         <v>2</v>
@@ -3801,18 +3909,18 @@
       <c r="ALX4" s="4"/>
       <c r="ALY4" s="4"/>
     </row>
-    <row r="5" spans="1:1013" ht="25.5">
-      <c r="A5" s="8">
+    <row r="5" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>49</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="E5" s="10">
         <v>2</v>
@@ -3825,13 +3933,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4">
         <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>1</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
@@ -4838,21 +4946,21 @@
       <c r="ALX5" s="4"/>
       <c r="ALY5" s="4"/>
     </row>
-    <row r="6" spans="1:1013" ht="38.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:1013" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>50</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="E6" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="11">
         <v>6</v>
@@ -4862,10 +4970,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="4">
         <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>2</v>
       </c>
       <c r="K6" s="4">
         <v>0</v>
@@ -5875,37 +5983,37 @@
       <c r="ALX6" s="4"/>
       <c r="ALY6" s="4"/>
     </row>
-    <row r="7" spans="1:1013" ht="25.5">
-      <c r="A7" s="8">
+    <row r="7" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>51</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="E7" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F7" s="11">
         <v>6</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I7" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J7" s="4">
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L7" s="4">
         <v>0</v>
@@ -6912,21 +7020,21 @@
       <c r="ALX7" s="4"/>
       <c r="ALY7" s="4"/>
     </row>
-    <row r="8" spans="1:1013" ht="25.5">
-      <c r="A8" s="8">
+    <row r="8" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>52</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="10">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="11">
         <v>6</v>
@@ -6939,13 +7047,13 @@
         <v>0</v>
       </c>
       <c r="J8" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="4">
         <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>1.5</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -7949,28 +8057,28 @@
       <c r="ALX8" s="4"/>
       <c r="ALY8" s="4"/>
     </row>
-    <row r="9" spans="1:1013" ht="25.5">
-      <c r="A9" s="8">
+    <row r="9" spans="1:1013" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>53</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="E9" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" s="11">
         <v>6</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="4">
         <v>0</v>
@@ -7979,7 +8087,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
@@ -8986,21 +9094,21 @@
       <c r="ALX9" s="4"/>
       <c r="ALY9" s="4"/>
     </row>
-    <row r="10" spans="1:1013" ht="25.5">
-      <c r="A10" s="8">
+    <row r="10" spans="1:1013" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>54</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="E10" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="11">
         <v>6</v>
@@ -9010,7 +9118,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="4">
         <v>0</v>
@@ -9019,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -10023,28 +10131,28 @@
       <c r="ALX10" s="4"/>
       <c r="ALY10" s="4"/>
     </row>
-    <row r="11" spans="1:1013" ht="25.5">
-      <c r="A11" s="8">
+    <row r="11" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>55</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="E11" s="10">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F11" s="11">
         <v>6</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="4">
         <v>0</v>
@@ -10053,7 +10161,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L11" s="4">
         <v>0</v>
@@ -11060,21 +11168,21 @@
       <c r="ALX11" s="4"/>
       <c r="ALY11" s="4"/>
     </row>
-    <row r="12" spans="1:1013">
-      <c r="A12" s="8">
+    <row r="12" spans="1:1013" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="E12" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" s="11">
         <v>6</v>
@@ -11084,13 +11192,13 @@
         <v>0</v>
       </c>
       <c r="I12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="4">
         <v>0</v>
@@ -12097,40 +12205,40 @@
       <c r="ALX12" s="4"/>
       <c r="ALY12" s="4"/>
     </row>
-    <row r="13" spans="1:1013" ht="25.5">
-      <c r="A13" s="8">
+    <row r="13" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>57</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="E13" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" s="11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -13134,19 +13242,41 @@
       <c r="ALX13" s="4"/>
       <c r="ALY13" s="4"/>
     </row>
-    <row r="14" spans="1:1013">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
+    <row r="14" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>58</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="10">
+        <v>7.5</v>
+      </c>
+      <c r="F14" s="11">
+        <v>7</v>
+      </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="H14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1.5</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -14149,19 +14279,41 @@
       <c r="ALX14" s="4"/>
       <c r="ALY14" s="4"/>
     </row>
-    <row r="15" spans="1:1013">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
+    <row r="15" spans="1:1013" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>59</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>4</v>
+      </c>
+      <c r="F15" s="11">
+        <v>7</v>
+      </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -15164,19 +15316,41 @@
       <c r="ALX15" s="4"/>
       <c r="ALY15" s="4"/>
     </row>
-    <row r="16" spans="1:1013">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
+    <row r="16" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>60</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="10">
+        <v>2</v>
+      </c>
+      <c r="F16" s="11">
+        <v>7</v>
+      </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2</v>
+      </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -16179,19 +16353,41 @@
       <c r="ALX16" s="4"/>
       <c r="ALY16" s="4"/>
     </row>
-    <row r="17" spans="1:1013">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
+    <row r="17" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>61</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="10">
+        <v>2</v>
+      </c>
+      <c r="F17" s="11">
+        <v>7</v>
+      </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="H17" s="4">
+        <v>2</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -17194,72 +17390,182 @@
       <c r="ALX17" s="4"/>
       <c r="ALY17" s="4"/>
     </row>
-    <row r="18" spans="1:1013">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+    <row r="18" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>62</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="10">
+        <v>3</v>
+      </c>
+      <c r="F18" s="11">
+        <v>7</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>3</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:1013">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+    <row r="19" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>63</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="10">
+        <v>9</v>
+      </c>
+      <c r="F19" s="11">
+        <v>7</v>
+      </c>
+      <c r="H19" s="4">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>3</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="1:1013">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+    <row r="20" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>64</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="11">
+        <v>7</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:1013">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+    <row r="21" spans="1:1013" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>65</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="10">
+        <v>2</v>
+      </c>
+      <c r="F21" s="11">
+        <v>7</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:1013">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+    <row r="22" spans="1:1013" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>66</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="10">
+        <v>5</v>
+      </c>
+      <c r="F22" s="11">
+        <v>7</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:1013">
+    <row r="23" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -17283,14 +17589,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.140625" style="5"/>
@@ -17298,7 +17604,7 @@
     <col min="1025" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30.75" customHeight="1">
+    <row r="1" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17309,7 +17615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>46</v>
       </c>
@@ -17321,7 +17627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>47</v>
       </c>
@@ -17333,72 +17639,72 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" s="12" customFormat="1">
+    <row r="5" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
       <c r="B5" s="4"/>
       <c r="C5" s="31"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" s="12" customFormat="1">
+    <row r="8" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="31"/>
       <c r="B8" s="4"/>
       <c r="C8" s="31"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -17414,14 +17720,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="23" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="21" customWidth="1"/>
@@ -17433,7 +17739,7 @@
     <col min="9" max="16384" width="11.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" ht="28.5">
+    <row r="1" spans="1:8" s="13" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>13</v>
       </c>
@@ -17459,7 +17765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="23">
         <v>41938</v>
       </c>
@@ -17486,7 +17792,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>41938</v>
       </c>
@@ -17513,7 +17819,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
       <c r="B5" s="21"/>
       <c r="C5" s="25"/>
@@ -17523,25 +17829,25 @@
       <c r="G5" s="26"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="22"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
       <c r="B9" s="29"/>
       <c r="C9" s="17"/>
@@ -17549,7 +17855,7 @@
       <c r="E9" s="22"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="28"/>
       <c r="B10" s="30"/>
       <c r="C10" s="17"/>
@@ -17558,7 +17864,7 @@
       <c r="F10" s="18"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="28"/>
       <c r="B11" s="30"/>
       <c r="C11" s="17"/>
@@ -17566,7 +17872,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="28"/>
       <c r="B12" s="30"/>
       <c r="C12" s="17"/>
@@ -17574,7 +17880,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="22"/>
       <c r="C13" s="17"/>
@@ -17582,7 +17888,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="22"/>
       <c r="C14" s="17"/>
@@ -17590,7 +17896,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="22"/>
       <c r="C15" s="17"/>
@@ -17598,7 +17904,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="22"/>
       <c r="C16" s="17"/>
@@ -17606,7 +17912,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="19" spans="1:8" s="12" customFormat="1">
+    <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24"/>
       <c r="B19" s="26"/>
       <c r="C19" s="25"/>
@@ -17616,7 +17922,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="22"/>
       <c r="C20" s="17"/>
@@ -17624,7 +17930,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="22"/>
       <c r="C21" s="17"/>
@@ -17632,7 +17938,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="22"/>
       <c r="C22" s="17"/>
@@ -17640,7 +17946,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="22"/>
       <c r="C23" s="17"/>
@@ -17648,7 +17954,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="22"/>
       <c r="C24" s="17"/>
@@ -17656,7 +17962,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="22"/>
       <c r="C25" s="17"/>
@@ -17664,7 +17970,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="18"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="22"/>
       <c r="C26" s="17"/>
@@ -17672,7 +17978,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="18"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="22"/>
       <c r="C27" s="17"/>
@@ -17680,7 +17986,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="22"/>
       <c r="C28" s="17"/>
@@ -17688,7 +17994,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="18"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="22"/>
       <c r="C29" s="17"/>
@@ -17696,7 +18002,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="18"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="22"/>
       <c r="C30" s="17"/>
@@ -17704,7 +18010,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="22"/>
       <c r="C31" s="17"/>
@@ -17712,7 +18018,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="18"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="22"/>
       <c r="C32" s="17"/>
@@ -17720,7 +18026,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="22"/>
       <c r="C33" s="17"/>
@@ -17728,7 +18034,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="18"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="22"/>
       <c r="C34" s="17"/>
@@ -17736,7 +18042,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="22"/>
       <c r="C35" s="17"/>

</xml_diff>